<commit_message>
project_pasteur_rest 2016-02-25 / 03 서버적용
</commit_message>
<xml_diff>
--- a/src/main/resources/static/EnergyLog.xlsx
+++ b/src/main/resources/static/EnergyLog.xlsx
@@ -320,9 +320,6 @@
     <t>전력량 탄소배출량</t>
   </si>
   <si>
-    <t xml:space="preserve"> 1(toe) = 0.00023(Kwh)</t>
-  </si>
-  <si>
     <t>합 계 (toe)</t>
   </si>
   <si>
@@ -1022,11 +1019,15 @@
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t>#{daily}</t>
+    <t xml:space="preserve"> (날씨 : #{d1012}  최고: #{d1013}℃,   최저:   #{d1014}℃ )</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> (날씨 : #{d1012}  최고: #{d1013}℃,   최저:   #{d1014}℃ )</t>
+    <t>1(toe) = 0.00023(Kwh)</t>
+    <phoneticPr fontId="13" type="noConversion"/>
+  </si>
+  <si>
+    <t>#{dailyText}</t>
     <phoneticPr fontId="13" type="noConversion"/>
   </si>
 </sst>
@@ -2304,240 +2305,6 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="29" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2562,8 +2329,242 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="56" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="62" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="67" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="69" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="70" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
@@ -2930,7 +2931,7 @@
   <dimension ref="A1:J82"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2941,18 +2942,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="44.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="135"/>
-      <c r="C1" s="135"/>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-      <c r="I1" s="135"/>
-      <c r="J1" s="135"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
     </row>
     <row r="2" spans="1:10" ht="21" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -2964,27 +2965,27 @@
       <c r="G2" s="2"/>
       <c r="H2" s="3"/>
       <c r="I2" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="23.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="128" t="s">
-        <v>324</v>
-      </c>
-      <c r="B3" s="128"/>
-      <c r="C3" s="128"/>
-      <c r="D3" s="141" t="s">
+      <c r="A3" s="75" t="s">
         <v>325</v>
       </c>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="63" t="s">
+        <v>323</v>
+      </c>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
       <c r="H3" s="6"/>
-      <c r="I3" s="136"/>
-      <c r="J3" s="136"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
     </row>
     <row r="4" spans="1:10" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="7"/>
@@ -2995,14 +2996,14 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="6"/>
-      <c r="I4" s="136"/>
-      <c r="J4" s="136"/>
+      <c r="I4" s="58"/>
+      <c r="J4" s="58"/>
     </row>
     <row r="5" spans="1:10" s="10" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="143" t="s">
-        <v>297</v>
-      </c>
-      <c r="B5" s="144"/>
+      <c r="A5" s="65" t="s">
+        <v>296</v>
+      </c>
+      <c r="B5" s="66"/>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -3013,10 +3014,10 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="129" t="s">
+      <c r="A6" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="129"/>
+      <c r="B6" s="76"/>
       <c r="C6" s="11" t="s">
         <v>2</v>
       </c>
@@ -3035,18 +3036,18 @@
       <c r="H6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I6" s="130" t="s">
+      <c r="I6" s="77" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="130"/>
+      <c r="J6" s="77"/>
     </row>
     <row r="7" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="131" t="s">
+      <c r="A7" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="132"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="14" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D7" s="14" t="s">
         <v>10</v>
@@ -3063,16 +3064,16 @@
       <c r="H7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I7" s="133" t="s">
+      <c r="I7" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="J7" s="134"/>
+      <c r="J7" s="81"/>
     </row>
     <row r="8" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="137" t="s">
+      <c r="A8" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="138"/>
+      <c r="B8" s="60"/>
       <c r="C8" s="15" t="s">
         <v>17</v>
       </c>
@@ -3091,16 +3092,16 @@
       <c r="H8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="139" t="s">
+      <c r="I8" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="140"/>
+      <c r="J8" s="62"/>
     </row>
     <row r="9" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="118" t="s">
+      <c r="A9" s="67" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="119"/>
+      <c r="B9" s="68"/>
       <c r="C9" s="16" t="s">
         <v>25</v>
       </c>
@@ -3119,10 +3120,10 @@
       <c r="H9" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="I9" s="120" t="s">
+      <c r="I9" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="J9" s="121"/>
+      <c r="J9" s="70"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17"/>
@@ -3137,12 +3138,12 @@
       <c r="J10" s="17"/>
     </row>
     <row r="11" spans="1:10" s="10" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="143" t="s">
-        <v>301</v>
-      </c>
-      <c r="B11" s="144"/>
-      <c r="C11" s="144"/>
-      <c r="D11" s="144"/>
+      <c r="A11" s="65" t="s">
+        <v>300</v>
+      </c>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
       <c r="E11" s="17"/>
       <c r="F11" s="17"/>
       <c r="G11" s="17"/>
@@ -3151,11 +3152,11 @@
       <c r="J11" s="17"/>
     </row>
     <row r="12" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="122" t="s">
+      <c r="A12" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="122"/>
-      <c r="C12" s="122"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
       <c r="D12" s="18" t="s">
         <v>33</v>
       </c>
@@ -3165,21 +3166,21 @@
       <c r="F12" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="122" t="s">
+      <c r="G12" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="H12" s="122"/>
-      <c r="I12" s="122"/>
-      <c r="J12" s="122"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
     </row>
     <row r="13" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="123" t="s">
+      <c r="A13" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="124" t="s">
+      <c r="B13" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="C13" s="124"/>
+      <c r="C13" s="83"/>
       <c r="D13" s="19" t="s">
         <v>39</v>
       </c>
@@ -3189,16 +3190,16 @@
       <c r="F13" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="116" t="s">
+      <c r="G13" s="71" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="116"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
+      <c r="H13" s="71"/>
+      <c r="I13" s="71"/>
+      <c r="J13" s="71"/>
     </row>
     <row r="14" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="123"/>
-      <c r="B14" s="125" t="s">
+      <c r="A14" s="72"/>
+      <c r="B14" s="84" t="s">
         <v>43</v>
       </c>
       <c r="C14" s="20" t="s">
@@ -3213,21 +3214,21 @@
       <c r="F14" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="116" t="s">
+      <c r="G14" s="71" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="116"/>
-      <c r="I14" s="116"/>
-      <c r="J14" s="116"/>
+      <c r="H14" s="71"/>
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
     </row>
     <row r="15" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="123"/>
-      <c r="B15" s="125"/>
+      <c r="A15" s="72"/>
+      <c r="B15" s="84"/>
       <c r="C15" s="21" t="s">
         <v>49</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>50</v>
@@ -3235,19 +3236,19 @@
       <c r="F15" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="G15" s="116" t="s">
+      <c r="G15" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="116"/>
-      <c r="I15" s="116"/>
-      <c r="J15" s="116"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
     </row>
     <row r="16" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="123"/>
-      <c r="B16" s="115" t="s">
+      <c r="A16" s="72"/>
+      <c r="B16" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="115"/>
+      <c r="C16" s="87"/>
       <c r="D16" s="19" t="s">
         <v>54</v>
       </c>
@@ -3257,17 +3258,17 @@
       <c r="F16" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="116" t="s">
+      <c r="G16" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="H16" s="116"/>
-      <c r="I16" s="116"/>
-      <c r="J16" s="116"/>
+      <c r="H16" s="71"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
     </row>
     <row r="17" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="123"/>
-      <c r="B17" s="126" t="s">
-        <v>303</v>
+      <c r="A17" s="72"/>
+      <c r="B17" s="89" t="s">
+        <v>302</v>
       </c>
       <c r="C17" s="22" t="s">
         <v>58</v>
@@ -3281,16 +3282,16 @@
       <c r="F17" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="116" t="s">
+      <c r="G17" s="71" t="s">
         <v>62</v>
       </c>
-      <c r="H17" s="116"/>
-      <c r="I17" s="116"/>
-      <c r="J17" s="116"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
     </row>
     <row r="18" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="123"/>
-      <c r="B18" s="126"/>
+      <c r="A18" s="72"/>
+      <c r="B18" s="89"/>
       <c r="C18" s="23" t="s">
         <v>63</v>
       </c>
@@ -3303,19 +3304,19 @@
       <c r="F18" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="116" t="s">
+      <c r="G18" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="H18" s="116"/>
-      <c r="I18" s="116"/>
-      <c r="J18" s="116"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
     </row>
     <row r="19" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="123"/>
-      <c r="B19" s="123" t="s">
+      <c r="A19" s="72"/>
+      <c r="B19" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="C19" s="123"/>
+      <c r="C19" s="72"/>
       <c r="D19" s="19" t="s">
         <v>69</v>
       </c>
@@ -3325,19 +3326,19 @@
       <c r="F19" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="116" t="s">
+      <c r="G19" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="H19" s="116"/>
-      <c r="I19" s="116"/>
-      <c r="J19" s="116"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="71"/>
+      <c r="J19" s="71"/>
     </row>
     <row r="20" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="123"/>
-      <c r="B20" s="123" t="s">
+      <c r="A20" s="72"/>
+      <c r="B20" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="123"/>
+      <c r="C20" s="72"/>
       <c r="D20" s="19" t="s">
         <v>74</v>
       </c>
@@ -3347,19 +3348,19 @@
       <c r="F20" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="G20" s="116" t="s">
+      <c r="G20" s="71" t="s">
         <v>77</v>
       </c>
-      <c r="H20" s="116"/>
-      <c r="I20" s="116"/>
-      <c r="J20" s="116"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="71"/>
+      <c r="J20" s="71"/>
     </row>
     <row r="21" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="123"/>
-      <c r="B21" s="127" t="s">
+      <c r="A21" s="72"/>
+      <c r="B21" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="127"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="19" t="s">
         <v>79</v>
       </c>
@@ -3369,21 +3370,21 @@
       <c r="F21" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="116" t="s">
+      <c r="G21" s="71" t="s">
         <v>82</v>
       </c>
-      <c r="H21" s="116"/>
-      <c r="I21" s="116"/>
-      <c r="J21" s="116"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="71"/>
+      <c r="J21" s="71"/>
     </row>
     <row r="22" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="114" t="s">
+      <c r="A22" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="115" t="s">
+      <c r="B22" s="87" t="s">
         <v>84</v>
       </c>
-      <c r="C22" s="115"/>
+      <c r="C22" s="87"/>
       <c r="D22" s="19" t="s">
         <v>85</v>
       </c>
@@ -3393,19 +3394,19 @@
       <c r="F22" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="G22" s="116" t="s">
+      <c r="G22" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="H22" s="116"/>
-      <c r="I22" s="116"/>
-      <c r="J22" s="116"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="71"/>
+      <c r="J22" s="71"/>
     </row>
     <row r="23" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="114"/>
-      <c r="B23" s="115" t="s">
+      <c r="A23" s="86"/>
+      <c r="B23" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="115"/>
+      <c r="C23" s="87"/>
       <c r="D23" s="19" t="s">
         <v>90</v>
       </c>
@@ -3415,120 +3416,120 @@
       <c r="F23" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="G23" s="116"/>
-      <c r="H23" s="116"/>
-      <c r="I23" s="116"/>
-      <c r="J23" s="116"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="71"/>
     </row>
     <row r="24" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="114" t="s">
+      <c r="A24" s="86" t="s">
         <v>92</v>
       </c>
-      <c r="B24" s="115" t="s">
+      <c r="B24" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="C24" s="115"/>
+      <c r="C24" s="87"/>
       <c r="D24" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>314</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="G24" s="88" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+    </row>
+    <row r="25" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="86"/>
+      <c r="B25" s="87" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="87"/>
+      <c r="D25" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="E24" s="19" t="s">
+      <c r="E25" s="19" t="s">
+        <v>313</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>321</v>
+      </c>
+      <c r="G25" s="88" t="s">
+        <v>96</v>
+      </c>
+      <c r="H25" s="88"/>
+      <c r="I25" s="88"/>
+      <c r="J25" s="88"/>
+    </row>
+    <row r="26" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="86"/>
+      <c r="B26" s="87" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" s="87"/>
+      <c r="D26" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="F24" s="19" t="s">
-        <v>323</v>
-      </c>
-      <c r="G24" s="117" t="s">
-        <v>94</v>
-      </c>
-      <c r="H24" s="117"/>
-      <c r="I24" s="117"/>
-      <c r="J24" s="117"/>
-    </row>
-    <row r="25" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="114"/>
-      <c r="B25" s="115" t="s">
-        <v>95</v>
-      </c>
-      <c r="C25" s="115"/>
-      <c r="D25" s="19" t="s">
-        <v>310</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>314</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>322</v>
-      </c>
-      <c r="G25" s="117" t="s">
-        <v>96</v>
-      </c>
-      <c r="H25" s="117"/>
-      <c r="I25" s="117"/>
-      <c r="J25" s="117"/>
-    </row>
-    <row r="26" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="114"/>
-      <c r="B26" s="115" t="s">
-        <v>97</v>
-      </c>
-      <c r="C26" s="115"/>
-      <c r="D26" s="19" t="s">
+      <c r="F26" s="19" t="s">
+        <v>320</v>
+      </c>
+      <c r="G26" s="88" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" s="88"/>
+      <c r="I26" s="88"/>
+      <c r="J26" s="88"/>
+    </row>
+    <row r="27" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="86"/>
+      <c r="B27" s="87" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" s="87"/>
+      <c r="D27" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="E26" s="19" t="s">
+      <c r="E27" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="F26" s="19" t="s">
-        <v>321</v>
-      </c>
-      <c r="G26" s="117" t="s">
-        <v>98</v>
-      </c>
-      <c r="H26" s="117"/>
-      <c r="I26" s="117"/>
-      <c r="J26" s="117"/>
-    </row>
-    <row r="27" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="114"/>
-      <c r="B27" s="115" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="115"/>
-      <c r="D27" s="19" t="s">
+      <c r="F27" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="G27" s="88" t="s">
+        <v>324</v>
+      </c>
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="88"/>
+    </row>
+    <row r="28" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="86"/>
+      <c r="B28" s="87" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" s="87"/>
+      <c r="D28" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E28" s="19" t="s">
         <v>317</v>
       </c>
-      <c r="F27" s="19" t="s">
-        <v>320</v>
-      </c>
-      <c r="G27" s="117" t="s">
-        <v>100</v>
-      </c>
-      <c r="H27" s="117"/>
-      <c r="I27" s="117"/>
-      <c r="J27" s="117"/>
-    </row>
-    <row r="28" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="114"/>
-      <c r="B28" s="115" t="s">
-        <v>101</v>
-      </c>
-      <c r="C28" s="115"/>
-      <c r="D28" s="19" t="s">
-        <v>313</v>
-      </c>
-      <c r="E28" s="19" t="s">
+      <c r="F28" s="19" t="s">
         <v>318</v>
       </c>
-      <c r="F28" s="19" t="s">
-        <v>319</v>
-      </c>
-      <c r="G28" s="116"/>
-      <c r="H28" s="116"/>
-      <c r="I28" s="116"/>
-      <c r="J28" s="116"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="71"/>
+      <c r="J28" s="71"/>
     </row>
     <row r="29" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17"/>
@@ -3543,13 +3544,13 @@
       <c r="J29" s="17"/>
     </row>
     <row r="30" spans="1:10" s="10" customFormat="1" ht="23.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="143" t="s">
-        <v>298</v>
-      </c>
-      <c r="B30" s="144"/>
-      <c r="C30" s="144"/>
-      <c r="D30" s="144"/>
-      <c r="E30" s="144"/>
+      <c r="A30" s="65" t="s">
+        <v>297</v>
+      </c>
+      <c r="B30" s="66"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="66"/>
+      <c r="E30" s="66"/>
       <c r="F30" s="17"/>
       <c r="G30" s="17"/>
       <c r="H30" s="17"/>
@@ -3558,147 +3559,147 @@
     </row>
     <row r="31" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="90" t="s">
         <v>102</v>
       </c>
-      <c r="B31" s="93" t="s">
+      <c r="C31" s="90"/>
+      <c r="D31" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C31" s="93"/>
-      <c r="D31" s="11" t="s">
+      <c r="E31" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="F31" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="F31" s="11" t="s">
+      <c r="G31" s="90" t="s">
         <v>106</v>
       </c>
-      <c r="G31" s="93" t="s">
-        <v>107</v>
-      </c>
-      <c r="H31" s="93"/>
-      <c r="I31" s="93"/>
-      <c r="J31" s="93"/>
+      <c r="H31" s="90"/>
+      <c r="I31" s="90"/>
+      <c r="J31" s="90"/>
     </row>
     <row r="32" spans="1:10" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B32" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="B32" s="99" t="s">
+      <c r="C32" s="92"/>
+      <c r="D32" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="100"/>
-      <c r="D32" s="25" t="s">
+      <c r="E32" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="25" t="s">
+      <c r="F32" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="F32" s="25" t="s">
+      <c r="G32" s="93" t="s">
         <v>112</v>
       </c>
-      <c r="G32" s="101" t="s">
-        <v>113</v>
-      </c>
-      <c r="H32" s="102"/>
-      <c r="I32" s="102"/>
-      <c r="J32" s="103"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="94"/>
+      <c r="J32" s="95"/>
     </row>
     <row r="33" spans="1:10" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" s="96" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="104" t="s">
+      <c r="C33" s="97"/>
+      <c r="D33" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C33" s="105"/>
-      <c r="D33" s="27" t="s">
+      <c r="E33" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="F33" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="F33" s="27" t="s">
+      <c r="G33" s="98" t="s">
         <v>118</v>
       </c>
-      <c r="G33" s="106" t="s">
-        <v>119</v>
-      </c>
-      <c r="H33" s="107"/>
-      <c r="I33" s="107"/>
-      <c r="J33" s="108"/>
+      <c r="H33" s="99"/>
+      <c r="I33" s="99"/>
+      <c r="J33" s="100"/>
     </row>
     <row r="34" spans="1:10" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="B34" s="101" t="s">
         <v>120</v>
       </c>
-      <c r="B34" s="109" t="s">
+      <c r="C34" s="102"/>
+      <c r="D34" s="29" t="s">
         <v>121</v>
       </c>
-      <c r="C34" s="110"/>
-      <c r="D34" s="29" t="s">
+      <c r="E34" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="E34" s="29" t="s">
+      <c r="F34" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="F34" s="29" t="s">
+      <c r="G34" s="103" t="s">
         <v>124</v>
       </c>
-      <c r="G34" s="111" t="s">
-        <v>125</v>
-      </c>
-      <c r="H34" s="112"/>
-      <c r="I34" s="112"/>
-      <c r="J34" s="113"/>
+      <c r="H34" s="104"/>
+      <c r="I34" s="104"/>
+      <c r="J34" s="105"/>
     </row>
     <row r="35" spans="1:10" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="101" t="s">
         <v>126</v>
       </c>
-      <c r="B35" s="109" t="s">
+      <c r="C35" s="102"/>
+      <c r="D35" s="29" t="s">
         <v>127</v>
       </c>
-      <c r="C35" s="110"/>
-      <c r="D35" s="29" t="s">
+      <c r="E35" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="E35" s="29" t="s">
+      <c r="F35" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="F35" s="29" t="s">
+      <c r="G35" s="103" t="s">
         <v>130</v>
       </c>
-      <c r="G35" s="111" t="s">
-        <v>131</v>
-      </c>
-      <c r="H35" s="112"/>
-      <c r="I35" s="112"/>
-      <c r="J35" s="113"/>
+      <c r="H35" s="104"/>
+      <c r="I35" s="104"/>
+      <c r="J35" s="105"/>
     </row>
     <row r="36" spans="1:10" s="13" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="30" t="s">
+        <v>131</v>
+      </c>
+      <c r="B36" s="106" t="s">
         <v>132</v>
       </c>
-      <c r="B36" s="88" t="s">
+      <c r="C36" s="107"/>
+      <c r="D36" s="31" t="s">
         <v>133</v>
       </c>
-      <c r="C36" s="89"/>
-      <c r="D36" s="31" t="s">
+      <c r="E36" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="F36" s="31" t="s">
         <v>135</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="G36" s="108" t="s">
         <v>136</v>
       </c>
-      <c r="G36" s="90" t="s">
-        <v>137</v>
-      </c>
-      <c r="H36" s="91"/>
-      <c r="I36" s="91"/>
-      <c r="J36" s="92"/>
+      <c r="H36" s="109"/>
+      <c r="I36" s="109"/>
+      <c r="J36" s="110"/>
     </row>
     <row r="37" spans="1:10" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="32"/>
@@ -3713,11 +3714,11 @@
       <c r="J37" s="35"/>
     </row>
     <row r="38" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="143" t="s">
-        <v>300</v>
-      </c>
-      <c r="B38" s="144"/>
-      <c r="C38" s="144"/>
+      <c r="A38" s="65" t="s">
+        <v>299</v>
+      </c>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
@@ -3728,652 +3729,652 @@
     </row>
     <row r="39" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="B39" s="93" t="s">
+        <v>101</v>
+      </c>
+      <c r="B39" s="90" t="s">
+        <v>137</v>
+      </c>
+      <c r="C39" s="90"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="90"/>
+      <c r="F39" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="C39" s="93"/>
-      <c r="D39" s="93"/>
-      <c r="E39" s="93"/>
-      <c r="F39" s="93" t="s">
+      <c r="G39" s="90"/>
+      <c r="H39" s="90"/>
+      <c r="I39" s="90"/>
+      <c r="J39" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="G39" s="93"/>
-      <c r="H39" s="93"/>
-      <c r="I39" s="93"/>
-      <c r="J39" s="11" t="s">
+    </row>
+    <row r="40" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="111" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="94" t="s">
+      <c r="B40" s="112" t="s">
         <v>141</v>
       </c>
-      <c r="B40" s="95" t="s">
+      <c r="C40" s="113"/>
+      <c r="D40" s="113"/>
+      <c r="E40" s="113"/>
+      <c r="F40" s="113" t="s">
         <v>142</v>
       </c>
-      <c r="C40" s="96"/>
-      <c r="D40" s="96"/>
-      <c r="E40" s="96"/>
-      <c r="F40" s="96" t="s">
+      <c r="G40" s="113"/>
+      <c r="H40" s="113"/>
+      <c r="I40" s="113"/>
+      <c r="J40" s="37" t="s">
         <v>143</v>
       </c>
-      <c r="G40" s="96"/>
-      <c r="H40" s="96"/>
-      <c r="I40" s="96"/>
-      <c r="J40" s="37" t="s">
+    </row>
+    <row r="41" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="111"/>
+      <c r="B41" s="114" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="94"/>
-      <c r="B41" s="97" t="s">
+      <c r="C41" s="115"/>
+      <c r="D41" s="115"/>
+      <c r="E41" s="115"/>
+      <c r="F41" s="115" t="s">
         <v>145</v>
       </c>
-      <c r="C41" s="86"/>
-      <c r="D41" s="86"/>
-      <c r="E41" s="86"/>
-      <c r="F41" s="86" t="s">
+      <c r="G41" s="115"/>
+      <c r="H41" s="115"/>
+      <c r="I41" s="115"/>
+      <c r="J41" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="G41" s="86"/>
-      <c r="H41" s="86"/>
-      <c r="I41" s="86"/>
-      <c r="J41" s="38" t="s">
+    </row>
+    <row r="42" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="111"/>
+      <c r="B42" s="114" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="42" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="94"/>
-      <c r="B42" s="97" t="s">
+      <c r="C42" s="115"/>
+      <c r="D42" s="115"/>
+      <c r="E42" s="115"/>
+      <c r="F42" s="115" t="s">
         <v>148</v>
       </c>
-      <c r="C42" s="86"/>
-      <c r="D42" s="86"/>
-      <c r="E42" s="86"/>
-      <c r="F42" s="86" t="s">
+      <c r="G42" s="115"/>
+      <c r="H42" s="115"/>
+      <c r="I42" s="115"/>
+      <c r="J42" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="G42" s="86"/>
-      <c r="H42" s="86"/>
-      <c r="I42" s="86"/>
-      <c r="J42" s="38" t="s">
+    </row>
+    <row r="43" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="111"/>
+      <c r="B43" s="114" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="94"/>
-      <c r="B43" s="97" t="s">
+      <c r="C43" s="115"/>
+      <c r="D43" s="115"/>
+      <c r="E43" s="115"/>
+      <c r="F43" s="115" t="s">
         <v>151</v>
       </c>
-      <c r="C43" s="86"/>
-      <c r="D43" s="86"/>
-      <c r="E43" s="86"/>
-      <c r="F43" s="86" t="s">
+      <c r="G43" s="115"/>
+      <c r="H43" s="115"/>
+      <c r="I43" s="115"/>
+      <c r="J43" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="G43" s="86"/>
-      <c r="H43" s="86"/>
-      <c r="I43" s="86"/>
-      <c r="J43" s="38" t="s">
+    </row>
+    <row r="44" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="111"/>
+      <c r="B44" s="114" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="94"/>
-      <c r="B44" s="97" t="s">
+      <c r="C44" s="115"/>
+      <c r="D44" s="115"/>
+      <c r="E44" s="115"/>
+      <c r="F44" s="115" t="s">
         <v>154</v>
       </c>
-      <c r="C44" s="86"/>
-      <c r="D44" s="86"/>
-      <c r="E44" s="86"/>
-      <c r="F44" s="86" t="s">
+      <c r="G44" s="115"/>
+      <c r="H44" s="115"/>
+      <c r="I44" s="115"/>
+      <c r="J44" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="G44" s="86"/>
-      <c r="H44" s="86"/>
-      <c r="I44" s="86"/>
-      <c r="J44" s="38" t="s">
+    </row>
+    <row r="45" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="111"/>
+      <c r="B45" s="114" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="94"/>
-      <c r="B45" s="97" t="s">
+      <c r="C45" s="115"/>
+      <c r="D45" s="115"/>
+      <c r="E45" s="115"/>
+      <c r="F45" s="115" t="s">
         <v>157</v>
       </c>
-      <c r="C45" s="86"/>
-      <c r="D45" s="86"/>
-      <c r="E45" s="86"/>
-      <c r="F45" s="86" t="s">
+      <c r="G45" s="115"/>
+      <c r="H45" s="115"/>
+      <c r="I45" s="115"/>
+      <c r="J45" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="G45" s="86"/>
-      <c r="H45" s="86"/>
-      <c r="I45" s="86"/>
-      <c r="J45" s="38" t="s">
+    </row>
+    <row r="46" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="111"/>
+      <c r="B46" s="114" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="46" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="94"/>
-      <c r="B46" s="97" t="s">
+      <c r="C46" s="115"/>
+      <c r="D46" s="115"/>
+      <c r="E46" s="115"/>
+      <c r="F46" s="115" t="s">
         <v>160</v>
       </c>
-      <c r="C46" s="86"/>
-      <c r="D46" s="86"/>
-      <c r="E46" s="86"/>
-      <c r="F46" s="86" t="s">
+      <c r="G46" s="115"/>
+      <c r="H46" s="115"/>
+      <c r="I46" s="115"/>
+      <c r="J46" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="G46" s="86"/>
-      <c r="H46" s="86"/>
-      <c r="I46" s="86"/>
-      <c r="J46" s="38" t="s">
+    </row>
+    <row r="47" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="111"/>
+      <c r="B47" s="114" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="94"/>
-      <c r="B47" s="97" t="s">
+      <c r="C47" s="115"/>
+      <c r="D47" s="115"/>
+      <c r="E47" s="115"/>
+      <c r="F47" s="115" t="s">
         <v>163</v>
       </c>
-      <c r="C47" s="86"/>
-      <c r="D47" s="86"/>
-      <c r="E47" s="86"/>
-      <c r="F47" s="86" t="s">
+      <c r="G47" s="115"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="115"/>
+      <c r="J47" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="G47" s="86"/>
-      <c r="H47" s="86"/>
-      <c r="I47" s="86"/>
-      <c r="J47" s="38" t="s">
+    </row>
+    <row r="48" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="111"/>
+      <c r="B48" s="114" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="48" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="94"/>
-      <c r="B48" s="97" t="s">
+      <c r="C48" s="115"/>
+      <c r="D48" s="115"/>
+      <c r="E48" s="115"/>
+      <c r="F48" s="115" t="s">
         <v>166</v>
       </c>
-      <c r="C48" s="86"/>
-      <c r="D48" s="86"/>
-      <c r="E48" s="86"/>
-      <c r="F48" s="86" t="s">
+      <c r="G48" s="115"/>
+      <c r="H48" s="115"/>
+      <c r="I48" s="115"/>
+      <c r="J48" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="G48" s="86"/>
-      <c r="H48" s="86"/>
-      <c r="I48" s="86"/>
-      <c r="J48" s="38" t="s">
+    </row>
+    <row r="49" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="111"/>
+      <c r="B49" s="116" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="49" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="94"/>
-      <c r="B49" s="98" t="s">
+      <c r="C49" s="117"/>
+      <c r="D49" s="117"/>
+      <c r="E49" s="117"/>
+      <c r="F49" s="117" t="s">
         <v>169</v>
       </c>
-      <c r="C49" s="84"/>
-      <c r="D49" s="84"/>
-      <c r="E49" s="84"/>
-      <c r="F49" s="84" t="s">
+      <c r="G49" s="117"/>
+      <c r="H49" s="117"/>
+      <c r="I49" s="117"/>
+      <c r="J49" s="39" t="s">
         <v>170</v>
       </c>
-      <c r="G49" s="84"/>
-      <c r="H49" s="84"/>
-      <c r="I49" s="84"/>
-      <c r="J49" s="39" t="s">
+    </row>
+    <row r="50" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="118" t="s">
+        <v>83</v>
+      </c>
+      <c r="B50" s="115" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="50" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="85" t="s">
-        <v>83</v>
-      </c>
-      <c r="B50" s="86" t="s">
+      <c r="C50" s="115"/>
+      <c r="D50" s="115"/>
+      <c r="E50" s="115"/>
+      <c r="F50" s="115" t="s">
         <v>172</v>
       </c>
-      <c r="C50" s="86"/>
-      <c r="D50" s="86"/>
-      <c r="E50" s="86"/>
-      <c r="F50" s="86" t="s">
+      <c r="G50" s="115"/>
+      <c r="H50" s="115"/>
+      <c r="I50" s="115"/>
+      <c r="J50" s="40" t="s">
         <v>173</v>
       </c>
-      <c r="G50" s="86"/>
-      <c r="H50" s="86"/>
-      <c r="I50" s="86"/>
-      <c r="J50" s="40" t="s">
+    </row>
+    <row r="51" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="118"/>
+      <c r="B51" s="115" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="51" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="85"/>
-      <c r="B51" s="86" t="s">
+      <c r="C51" s="115"/>
+      <c r="D51" s="115"/>
+      <c r="E51" s="115"/>
+      <c r="F51" s="115" t="s">
         <v>175</v>
       </c>
-      <c r="C51" s="86"/>
-      <c r="D51" s="86"/>
-      <c r="E51" s="86"/>
-      <c r="F51" s="86" t="s">
+      <c r="G51" s="115"/>
+      <c r="H51" s="115"/>
+      <c r="I51" s="115"/>
+      <c r="J51" s="40" t="s">
         <v>176</v>
       </c>
-      <c r="G51" s="86"/>
-      <c r="H51" s="86"/>
-      <c r="I51" s="86"/>
-      <c r="J51" s="40" t="s">
+    </row>
+    <row r="52" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="118"/>
+      <c r="B52" s="115" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="52" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="85"/>
-      <c r="B52" s="86" t="s">
+      <c r="C52" s="115"/>
+      <c r="D52" s="115"/>
+      <c r="E52" s="115"/>
+      <c r="F52" s="115" t="s">
         <v>178</v>
       </c>
-      <c r="C52" s="86"/>
-      <c r="D52" s="86"/>
-      <c r="E52" s="86"/>
-      <c r="F52" s="86" t="s">
+      <c r="G52" s="115"/>
+      <c r="H52" s="115"/>
+      <c r="I52" s="115"/>
+      <c r="J52" s="40" t="s">
         <v>179</v>
       </c>
-      <c r="G52" s="86"/>
-      <c r="H52" s="86"/>
-      <c r="I52" s="86"/>
-      <c r="J52" s="40" t="s">
+    </row>
+    <row r="53" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="118"/>
+      <c r="B53" s="115" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="53" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="85"/>
-      <c r="B53" s="86" t="s">
+      <c r="C53" s="115"/>
+      <c r="D53" s="115"/>
+      <c r="E53" s="115"/>
+      <c r="F53" s="115" t="s">
         <v>181</v>
       </c>
-      <c r="C53" s="86"/>
-      <c r="D53" s="86"/>
-      <c r="E53" s="86"/>
-      <c r="F53" s="86" t="s">
+      <c r="G53" s="115"/>
+      <c r="H53" s="115"/>
+      <c r="I53" s="115"/>
+      <c r="J53" s="40" t="s">
         <v>182</v>
       </c>
-      <c r="G53" s="86"/>
-      <c r="H53" s="86"/>
-      <c r="I53" s="86"/>
-      <c r="J53" s="40" t="s">
+    </row>
+    <row r="54" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="118"/>
+      <c r="B54" s="115" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="54" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="85"/>
-      <c r="B54" s="86" t="s">
+      <c r="C54" s="115"/>
+      <c r="D54" s="115"/>
+      <c r="E54" s="115"/>
+      <c r="F54" s="115" t="s">
         <v>184</v>
       </c>
-      <c r="C54" s="86"/>
-      <c r="D54" s="86"/>
-      <c r="E54" s="86"/>
-      <c r="F54" s="86" t="s">
+      <c r="G54" s="115"/>
+      <c r="H54" s="115"/>
+      <c r="I54" s="115"/>
+      <c r="J54" s="40" t="s">
         <v>185</v>
       </c>
-      <c r="G54" s="86"/>
-      <c r="H54" s="86"/>
-      <c r="I54" s="86"/>
-      <c r="J54" s="40" t="s">
+    </row>
+    <row r="55" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="118"/>
+      <c r="B55" s="115" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="55" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="85"/>
-      <c r="B55" s="86" t="s">
+      <c r="C55" s="115"/>
+      <c r="D55" s="115"/>
+      <c r="E55" s="115"/>
+      <c r="F55" s="115" t="s">
         <v>187</v>
       </c>
-      <c r="C55" s="86"/>
-      <c r="D55" s="86"/>
-      <c r="E55" s="86"/>
-      <c r="F55" s="86" t="s">
+      <c r="G55" s="115"/>
+      <c r="H55" s="115"/>
+      <c r="I55" s="115"/>
+      <c r="J55" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="G55" s="86"/>
-      <c r="H55" s="86"/>
-      <c r="I55" s="86"/>
-      <c r="J55" s="40" t="s">
+    </row>
+    <row r="56" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="118"/>
+      <c r="B56" s="115" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="56" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="85"/>
-      <c r="B56" s="86" t="s">
+      <c r="C56" s="115"/>
+      <c r="D56" s="115"/>
+      <c r="E56" s="115"/>
+      <c r="F56" s="115" t="s">
         <v>190</v>
       </c>
-      <c r="C56" s="86"/>
-      <c r="D56" s="86"/>
-      <c r="E56" s="86"/>
-      <c r="F56" s="86" t="s">
+      <c r="G56" s="115"/>
+      <c r="H56" s="115"/>
+      <c r="I56" s="115"/>
+      <c r="J56" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="G56" s="86"/>
-      <c r="H56" s="86"/>
-      <c r="I56" s="86"/>
-      <c r="J56" s="40" t="s">
+    </row>
+    <row r="57" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="118"/>
+      <c r="B57" s="115" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="57" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="85"/>
-      <c r="B57" s="86" t="s">
+      <c r="C57" s="115"/>
+      <c r="D57" s="115"/>
+      <c r="E57" s="115"/>
+      <c r="F57" s="115" t="s">
         <v>193</v>
       </c>
-      <c r="C57" s="86"/>
-      <c r="D57" s="86"/>
-      <c r="E57" s="86"/>
-      <c r="F57" s="86" t="s">
+      <c r="G57" s="115"/>
+      <c r="H57" s="115"/>
+      <c r="I57" s="115"/>
+      <c r="J57" s="40" t="s">
         <v>194</v>
       </c>
-      <c r="G57" s="86"/>
-      <c r="H57" s="86"/>
-      <c r="I57" s="86"/>
-      <c r="J57" s="40" t="s">
+    </row>
+    <row r="58" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="118"/>
+      <c r="B58" s="115" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="58" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="85"/>
-      <c r="B58" s="86" t="s">
+      <c r="C58" s="115"/>
+      <c r="D58" s="115"/>
+      <c r="E58" s="115"/>
+      <c r="F58" s="115" t="s">
         <v>196</v>
       </c>
-      <c r="C58" s="86"/>
-      <c r="D58" s="86"/>
-      <c r="E58" s="86"/>
-      <c r="F58" s="86" t="s">
+      <c r="G58" s="115"/>
+      <c r="H58" s="115"/>
+      <c r="I58" s="115"/>
+      <c r="J58" s="40" t="s">
         <v>197</v>
       </c>
-      <c r="G58" s="86"/>
-      <c r="H58" s="86"/>
-      <c r="I58" s="86"/>
-      <c r="J58" s="40" t="s">
+    </row>
+    <row r="59" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="118"/>
+      <c r="B59" s="119" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="59" spans="1:10" s="13" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="85"/>
-      <c r="B59" s="87" t="s">
+      <c r="C59" s="119"/>
+      <c r="D59" s="119"/>
+      <c r="E59" s="119"/>
+      <c r="F59" s="119" t="s">
         <v>199</v>
       </c>
-      <c r="C59" s="87"/>
-      <c r="D59" s="87"/>
-      <c r="E59" s="87"/>
-      <c r="F59" s="87" t="s">
+      <c r="G59" s="119"/>
+      <c r="H59" s="119"/>
+      <c r="I59" s="119"/>
+      <c r="J59" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="G59" s="87"/>
-      <c r="H59" s="87"/>
-      <c r="I59" s="87"/>
-      <c r="J59" s="41" t="s">
+    </row>
+    <row r="60" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="124" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="60" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="81" t="s">
+      <c r="B60" s="127" t="s">
         <v>202</v>
       </c>
-      <c r="B60" s="82" t="s">
+      <c r="C60" s="127"/>
+      <c r="D60" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="C60" s="82"/>
-      <c r="D60" s="42" t="s">
+      <c r="E60" s="43" t="s">
         <v>204</v>
       </c>
-      <c r="E60" s="43" t="s">
+      <c r="F60" s="42" t="s">
         <v>205</v>
       </c>
-      <c r="F60" s="42" t="s">
+      <c r="G60" s="128" t="s">
         <v>206</v>
       </c>
-      <c r="G60" s="83" t="s">
+      <c r="H60" s="128"/>
+      <c r="I60" s="128"/>
+      <c r="J60" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="H60" s="83"/>
-      <c r="I60" s="83"/>
-      <c r="J60" s="44" t="s">
+    </row>
+    <row r="61" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="125"/>
+      <c r="B61" s="120" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="61" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="57"/>
-      <c r="B61" s="79" t="s">
+      <c r="C61" s="120"/>
+      <c r="D61" s="45" t="s">
         <v>209</v>
       </c>
-      <c r="C61" s="79"/>
-      <c r="D61" s="45" t="s">
+      <c r="E61" s="45" t="s">
         <v>210</v>
       </c>
-      <c r="E61" s="45" t="s">
+      <c r="F61" s="45" t="s">
         <v>211</v>
       </c>
-      <c r="F61" s="45" t="s">
+      <c r="G61" s="120" t="s">
         <v>212</v>
       </c>
-      <c r="G61" s="79" t="s">
+      <c r="H61" s="120"/>
+      <c r="I61" s="120"/>
+      <c r="J61" s="46" t="s">
         <v>213</v>
       </c>
-      <c r="H61" s="79"/>
-      <c r="I61" s="79"/>
-      <c r="J61" s="46" t="s">
+    </row>
+    <row r="62" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="125"/>
+      <c r="B62" s="120" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="62" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="57"/>
-      <c r="B62" s="79" t="s">
+      <c r="C62" s="120"/>
+      <c r="D62" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="C62" s="79"/>
-      <c r="D62" s="45" t="s">
+      <c r="E62" s="45" t="s">
         <v>216</v>
       </c>
-      <c r="E62" s="45" t="s">
+      <c r="F62" s="45" t="s">
         <v>217</v>
       </c>
-      <c r="F62" s="45" t="s">
+      <c r="G62" s="120" t="s">
         <v>218</v>
       </c>
-      <c r="G62" s="79" t="s">
+      <c r="H62" s="120"/>
+      <c r="I62" s="120"/>
+      <c r="J62" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="H62" s="79"/>
-      <c r="I62" s="79"/>
-      <c r="J62" s="46" t="s">
+    </row>
+    <row r="63" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="125"/>
+      <c r="B63" s="120" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="63" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="57"/>
-      <c r="B63" s="79" t="s">
+      <c r="C63" s="120"/>
+      <c r="D63" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="C63" s="79"/>
-      <c r="D63" s="45" t="s">
+      <c r="E63" s="45" t="s">
         <v>222</v>
       </c>
-      <c r="E63" s="45" t="s">
+      <c r="F63" s="45" t="s">
         <v>223</v>
       </c>
-      <c r="F63" s="45" t="s">
+      <c r="G63" s="120" t="s">
         <v>224</v>
       </c>
-      <c r="G63" s="79" t="s">
+      <c r="H63" s="120"/>
+      <c r="I63" s="120"/>
+      <c r="J63" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="H63" s="79"/>
-      <c r="I63" s="79"/>
-      <c r="J63" s="46" t="s">
+    </row>
+    <row r="64" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="125"/>
+      <c r="B64" s="120" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="64" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="57"/>
-      <c r="B64" s="79" t="s">
+      <c r="C64" s="120"/>
+      <c r="D64" s="45" t="s">
         <v>227</v>
       </c>
-      <c r="C64" s="79"/>
-      <c r="D64" s="45" t="s">
+      <c r="E64" s="45" t="s">
         <v>228</v>
       </c>
-      <c r="E64" s="45" t="s">
+      <c r="F64" s="45" t="s">
         <v>229</v>
       </c>
-      <c r="F64" s="45" t="s">
+      <c r="G64" s="120" t="s">
         <v>230</v>
       </c>
-      <c r="G64" s="79" t="s">
+      <c r="H64" s="120"/>
+      <c r="I64" s="120"/>
+      <c r="J64" s="46" t="s">
         <v>231</v>
       </c>
-      <c r="H64" s="79"/>
-      <c r="I64" s="79"/>
-      <c r="J64" s="46" t="s">
+    </row>
+    <row r="65" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="125"/>
+      <c r="B65" s="120" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="65" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="57"/>
-      <c r="B65" s="79" t="s">
+      <c r="C65" s="120"/>
+      <c r="D65" s="45" t="s">
         <v>233</v>
       </c>
-      <c r="C65" s="79"/>
-      <c r="D65" s="45" t="s">
+      <c r="E65" s="45" t="s">
         <v>234</v>
       </c>
-      <c r="E65" s="45" t="s">
+      <c r="F65" s="45" t="s">
         <v>235</v>
       </c>
-      <c r="F65" s="45" t="s">
+      <c r="G65" s="120" t="s">
         <v>236</v>
       </c>
-      <c r="G65" s="79" t="s">
+      <c r="H65" s="120"/>
+      <c r="I65" s="120"/>
+      <c r="J65" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="H65" s="79"/>
-      <c r="I65" s="79"/>
-      <c r="J65" s="46" t="s">
+    </row>
+    <row r="66" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="125"/>
+      <c r="B66" s="120" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="66" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="57"/>
-      <c r="B66" s="79" t="s">
+      <c r="C66" s="120"/>
+      <c r="D66" s="45" t="s">
         <v>239</v>
       </c>
-      <c r="C66" s="79"/>
-      <c r="D66" s="45" t="s">
+      <c r="E66" s="45" t="s">
         <v>240</v>
       </c>
-      <c r="E66" s="45" t="s">
+      <c r="F66" s="45" t="s">
         <v>241</v>
       </c>
-      <c r="F66" s="45" t="s">
+      <c r="G66" s="120" t="s">
         <v>242</v>
       </c>
-      <c r="G66" s="79" t="s">
+      <c r="H66" s="120"/>
+      <c r="I66" s="120"/>
+      <c r="J66" s="46" t="s">
         <v>243</v>
       </c>
-      <c r="H66" s="79"/>
-      <c r="I66" s="79"/>
-      <c r="J66" s="46" t="s">
+    </row>
+    <row r="67" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="125"/>
+      <c r="B67" s="120" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="67" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="57"/>
-      <c r="B67" s="79" t="s">
+      <c r="C67" s="120"/>
+      <c r="D67" s="45" t="s">
         <v>245</v>
       </c>
-      <c r="C67" s="79"/>
-      <c r="D67" s="45" t="s">
+      <c r="E67" s="45" t="s">
         <v>246</v>
       </c>
-      <c r="E67" s="45" t="s">
+      <c r="F67" s="45" t="s">
         <v>247</v>
       </c>
-      <c r="F67" s="45" t="s">
+      <c r="G67" s="120" t="s">
         <v>248</v>
       </c>
-      <c r="G67" s="79" t="s">
+      <c r="H67" s="120"/>
+      <c r="I67" s="120"/>
+      <c r="J67" s="46" t="s">
         <v>249</v>
       </c>
-      <c r="H67" s="79"/>
-      <c r="I67" s="79"/>
-      <c r="J67" s="46" t="s">
+    </row>
+    <row r="68" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="125"/>
+      <c r="B68" s="120" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="68" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="57"/>
-      <c r="B68" s="79" t="s">
+      <c r="C68" s="120"/>
+      <c r="D68" s="45" t="s">
         <v>251</v>
       </c>
-      <c r="C68" s="79"/>
-      <c r="D68" s="45" t="s">
+      <c r="E68" s="45" t="s">
         <v>252</v>
       </c>
-      <c r="E68" s="45" t="s">
+      <c r="F68" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="F68" s="45" t="s">
+      <c r="G68" s="120" t="s">
         <v>254</v>
       </c>
-      <c r="G68" s="79" t="s">
+      <c r="H68" s="120"/>
+      <c r="I68" s="120"/>
+      <c r="J68" s="46" t="s">
         <v>255</v>
       </c>
-      <c r="H68" s="79"/>
-      <c r="I68" s="79"/>
-      <c r="J68" s="46" t="s">
+    </row>
+    <row r="69" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="125"/>
+      <c r="B69" s="120" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="57"/>
-      <c r="B69" s="79" t="s">
+      <c r="C69" s="120"/>
+      <c r="D69" s="45" t="s">
         <v>257</v>
       </c>
-      <c r="C69" s="79"/>
-      <c r="D69" s="45" t="s">
+      <c r="E69" s="45" t="s">
         <v>258</v>
       </c>
-      <c r="E69" s="45" t="s">
+      <c r="F69" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="F69" s="45" t="s">
+      <c r="G69" s="120" t="s">
         <v>260</v>
       </c>
-      <c r="G69" s="79" t="s">
+      <c r="H69" s="120"/>
+      <c r="I69" s="120"/>
+      <c r="J69" s="46" t="s">
         <v>261</v>
       </c>
-      <c r="H69" s="79"/>
-      <c r="I69" s="79"/>
-      <c r="J69" s="46" t="s">
+    </row>
+    <row r="70" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="126"/>
+      <c r="B70" s="121" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="70" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="58"/>
-      <c r="B70" s="80" t="s">
+      <c r="C70" s="121"/>
+      <c r="D70" s="47" t="s">
         <v>263</v>
       </c>
-      <c r="C70" s="80"/>
-      <c r="D70" s="47" t="s">
+      <c r="E70" s="47" t="s">
         <v>264</v>
       </c>
-      <c r="E70" s="47" t="s">
+      <c r="F70" s="47" t="s">
         <v>265</v>
       </c>
-      <c r="F70" s="47" t="s">
+      <c r="G70" s="121" t="s">
         <v>266</v>
       </c>
-      <c r="G70" s="80" t="s">
+      <c r="H70" s="121"/>
+      <c r="I70" s="121"/>
+      <c r="J70" s="48" t="s">
         <v>267</v>
-      </c>
-      <c r="H70" s="80"/>
-      <c r="I70" s="80"/>
-      <c r="J70" s="48" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="71" spans="1:10" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4389,11 +4390,11 @@
       <c r="J71" s="35"/>
     </row>
     <row r="72" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="145" t="s">
-        <v>299</v>
-      </c>
-      <c r="B72" s="146"/>
-      <c r="C72" s="146"/>
+      <c r="A72" s="73" t="s">
+        <v>298</v>
+      </c>
+      <c r="B72" s="74"/>
+      <c r="C72" s="74"/>
       <c r="D72" s="49"/>
       <c r="E72" s="49"/>
       <c r="F72" s="49"/>
@@ -4404,302 +4405,212 @@
     </row>
     <row r="73" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A73" s="50" t="s">
-        <v>102</v>
-      </c>
-      <c r="B73" s="66" t="s">
+        <v>101</v>
+      </c>
+      <c r="B73" s="134" t="s">
+        <v>268</v>
+      </c>
+      <c r="C73" s="134"/>
+      <c r="D73" s="134"/>
+      <c r="E73" s="134"/>
+      <c r="F73" s="134" t="s">
         <v>269</v>
       </c>
-      <c r="C73" s="66"/>
-      <c r="D73" s="66"/>
-      <c r="E73" s="66"/>
-      <c r="F73" s="66" t="s">
+      <c r="G73" s="134"/>
+      <c r="H73" s="134"/>
+      <c r="I73" s="134"/>
+      <c r="J73" s="135"/>
+    </row>
+    <row r="74" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="139" t="s">
+        <v>140</v>
+      </c>
+      <c r="B74" s="140" t="s">
         <v>270</v>
       </c>
-      <c r="G73" s="66"/>
-      <c r="H73" s="66"/>
-      <c r="I73" s="66"/>
-      <c r="J73" s="67"/>
-    </row>
-    <row r="74" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
-      <c r="A74" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="B74" s="72" t="s">
+      <c r="C74" s="141"/>
+      <c r="D74" s="141"/>
+      <c r="E74" s="141"/>
+      <c r="F74" s="142" t="s">
         <v>271</v>
       </c>
-      <c r="C74" s="73"/>
-      <c r="D74" s="73"/>
-      <c r="E74" s="73"/>
-      <c r="F74" s="74" t="s">
+      <c r="G74" s="142"/>
+      <c r="H74" s="142"/>
+      <c r="I74" s="142"/>
+      <c r="J74" s="143"/>
+    </row>
+    <row r="75" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="139"/>
+      <c r="B75" s="144" t="s">
         <v>272</v>
       </c>
-      <c r="G74" s="74"/>
-      <c r="H74" s="74"/>
-      <c r="I74" s="74"/>
-      <c r="J74" s="75"/>
-    </row>
-    <row r="75" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A75" s="71"/>
-      <c r="B75" s="76" t="s">
+      <c r="C75" s="133"/>
+      <c r="D75" s="133"/>
+      <c r="E75" s="133"/>
+      <c r="F75" s="122" t="s">
         <v>273</v>
       </c>
-      <c r="C75" s="65"/>
-      <c r="D75" s="65"/>
-      <c r="E75" s="65"/>
-      <c r="F75" s="61" t="s">
+      <c r="G75" s="122"/>
+      <c r="H75" s="122"/>
+      <c r="I75" s="122"/>
+      <c r="J75" s="123"/>
+    </row>
+    <row r="76" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="139"/>
+      <c r="B76" s="145" t="s">
         <v>274</v>
       </c>
-      <c r="G75" s="61"/>
-      <c r="H75" s="61"/>
-      <c r="I75" s="61"/>
-      <c r="J75" s="62"/>
-    </row>
-    <row r="76" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="71"/>
-      <c r="B76" s="77" t="s">
+      <c r="C76" s="146"/>
+      <c r="D76" s="146"/>
+      <c r="E76" s="146"/>
+      <c r="F76" s="131" t="s">
         <v>275</v>
       </c>
-      <c r="C76" s="78"/>
-      <c r="D76" s="78"/>
-      <c r="E76" s="78"/>
-      <c r="F76" s="63" t="s">
+      <c r="G76" s="131"/>
+      <c r="H76" s="131"/>
+      <c r="I76" s="131"/>
+      <c r="J76" s="132"/>
+    </row>
+    <row r="77" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="125" t="s">
+        <v>83</v>
+      </c>
+      <c r="B77" s="136" t="s">
         <v>276</v>
       </c>
-      <c r="G76" s="63"/>
-      <c r="H76" s="63"/>
-      <c r="I76" s="63"/>
-      <c r="J76" s="64"/>
-    </row>
-    <row r="77" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77" s="68" t="s">
+      <c r="C77" s="136"/>
+      <c r="D77" s="136"/>
+      <c r="E77" s="136"/>
+      <c r="F77" s="137" t="s">
         <v>277</v>
       </c>
-      <c r="C77" s="68"/>
-      <c r="D77" s="68"/>
-      <c r="E77" s="68"/>
-      <c r="F77" s="69" t="s">
+      <c r="G77" s="137"/>
+      <c r="H77" s="137"/>
+      <c r="I77" s="137"/>
+      <c r="J77" s="138"/>
+    </row>
+    <row r="78" spans="1:10" s="13" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="125"/>
+      <c r="B78" s="133" t="s">
         <v>278</v>
       </c>
-      <c r="G77" s="69"/>
-      <c r="H77" s="69"/>
-      <c r="I77" s="69"/>
-      <c r="J77" s="70"/>
-    </row>
-    <row r="78" spans="1:10" s="13" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="57"/>
-      <c r="B78" s="65" t="s">
+      <c r="C78" s="133"/>
+      <c r="D78" s="133"/>
+      <c r="E78" s="133"/>
+      <c r="F78" s="122" t="s">
         <v>279</v>
       </c>
-      <c r="C78" s="65"/>
-      <c r="D78" s="65"/>
-      <c r="E78" s="65"/>
-      <c r="F78" s="61" t="s">
+      <c r="G78" s="122"/>
+      <c r="H78" s="122"/>
+      <c r="I78" s="122"/>
+      <c r="J78" s="123"/>
+    </row>
+    <row r="79" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="125"/>
+      <c r="B79" s="133" t="s">
         <v>280</v>
       </c>
-      <c r="G78" s="61"/>
-      <c r="H78" s="61"/>
-      <c r="I78" s="61"/>
-      <c r="J78" s="62"/>
-    </row>
-    <row r="79" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="57"/>
-      <c r="B79" s="65" t="s">
+      <c r="C79" s="133"/>
+      <c r="D79" s="133"/>
+      <c r="E79" s="133"/>
+      <c r="F79" s="122" t="s">
         <v>281</v>
       </c>
-      <c r="C79" s="65"/>
-      <c r="D79" s="65"/>
-      <c r="E79" s="65"/>
-      <c r="F79" s="61" t="s">
+      <c r="G79" s="122"/>
+      <c r="H79" s="122"/>
+      <c r="I79" s="122"/>
+      <c r="J79" s="123"/>
+    </row>
+    <row r="80" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="125" t="s">
         <v>282</v>
       </c>
-      <c r="G79" s="61"/>
-      <c r="H79" s="61"/>
-      <c r="I79" s="61"/>
-      <c r="J79" s="62"/>
-    </row>
-    <row r="80" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="57" t="s">
+      <c r="B80" s="51" t="s">
         <v>283</v>
       </c>
-      <c r="B80" s="51" t="s">
+      <c r="C80" s="52" t="s">
         <v>284</v>
       </c>
-      <c r="C80" s="52" t="s">
+      <c r="D80" s="53" t="s">
         <v>285</v>
       </c>
-      <c r="D80" s="53" t="s">
+      <c r="E80" s="53" t="s">
         <v>286</v>
       </c>
-      <c r="E80" s="53" t="s">
+      <c r="F80" s="129" t="s">
         <v>287</v>
       </c>
-      <c r="F80" s="59" t="s">
+      <c r="G80" s="129"/>
+      <c r="H80" s="129"/>
+      <c r="I80" s="129"/>
+      <c r="J80" s="130"/>
+    </row>
+    <row r="81" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="125"/>
+      <c r="B81" s="52" t="s">
         <v>288</v>
       </c>
-      <c r="G80" s="59"/>
-      <c r="H80" s="59"/>
-      <c r="I80" s="59"/>
-      <c r="J80" s="60"/>
-    </row>
-    <row r="81" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="57"/>
-      <c r="B81" s="52" t="s">
+      <c r="C81" s="54" t="s">
         <v>289</v>
       </c>
-      <c r="C81" s="54" t="s">
+      <c r="D81" s="54" t="s">
         <v>290</v>
       </c>
-      <c r="D81" s="54" t="s">
+      <c r="E81" s="54" t="s">
         <v>291</v>
       </c>
-      <c r="E81" s="54" t="s">
+      <c r="F81" s="122" t="s">
         <v>292</v>
       </c>
-      <c r="F81" s="61" t="s">
+      <c r="G81" s="122"/>
+      <c r="H81" s="122"/>
+      <c r="I81" s="122"/>
+      <c r="J81" s="123"/>
+    </row>
+    <row r="82" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="126"/>
+      <c r="B82" s="55" t="s">
         <v>293</v>
       </c>
-      <c r="G81" s="61"/>
-      <c r="H81" s="61"/>
-      <c r="I81" s="61"/>
-      <c r="J81" s="62"/>
-    </row>
-    <row r="82" spans="1:10" s="13" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="58"/>
-      <c r="B82" s="55" t="s">
+      <c r="C82" s="56" t="s">
+        <v>303</v>
+      </c>
+      <c r="D82" s="56" t="s">
+        <v>304</v>
+      </c>
+      <c r="E82" s="56" t="s">
+        <v>305</v>
+      </c>
+      <c r="F82" s="131" t="s">
         <v>294</v>
       </c>
-      <c r="C82" s="56" t="s">
-        <v>304</v>
-      </c>
-      <c r="D82" s="56" t="s">
-        <v>305</v>
-      </c>
-      <c r="E82" s="56" t="s">
-        <v>306</v>
-      </c>
-      <c r="F82" s="63" t="s">
-        <v>295</v>
-      </c>
-      <c r="G82" s="63"/>
-      <c r="H82" s="63"/>
-      <c r="I82" s="63"/>
-      <c r="J82" s="64"/>
+      <c r="G82" s="131"/>
+      <c r="H82" s="131"/>
+      <c r="I82" s="131"/>
+      <c r="J82" s="132"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="152">
-    <mergeCell ref="A30:E30"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A72:C72"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="A13:A21"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="G19:J19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="G21:J21"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="G22:J22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="G23:J23"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="G24:J24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="A40:A49"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="F44:I44"/>
-    <mergeCell ref="B45:E45"/>
-    <mergeCell ref="F45:I45"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="F46:I46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="F47:I47"/>
-    <mergeCell ref="B48:E48"/>
-    <mergeCell ref="F48:I48"/>
-    <mergeCell ref="B49:E49"/>
-    <mergeCell ref="F49:I49"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="F50:I50"/>
-    <mergeCell ref="B51:E51"/>
-    <mergeCell ref="F51:I51"/>
-    <mergeCell ref="B52:E52"/>
-    <mergeCell ref="F52:I52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="F53:I53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="F54:I54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="F55:I55"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="F56:I56"/>
-    <mergeCell ref="B57:E57"/>
-    <mergeCell ref="F57:I57"/>
-    <mergeCell ref="B58:E58"/>
-    <mergeCell ref="F58:I58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="A80:A82"/>
+    <mergeCell ref="F80:J80"/>
+    <mergeCell ref="F81:J81"/>
+    <mergeCell ref="F82:J82"/>
+    <mergeCell ref="A77:A79"/>
+    <mergeCell ref="B79:E79"/>
+    <mergeCell ref="F79:J79"/>
+    <mergeCell ref="B73:E73"/>
+    <mergeCell ref="F73:J73"/>
+    <mergeCell ref="B77:E77"/>
+    <mergeCell ref="F77:J77"/>
+    <mergeCell ref="B78:E78"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="F74:J74"/>
+    <mergeCell ref="B75:E75"/>
+    <mergeCell ref="F75:J75"/>
+    <mergeCell ref="B76:E76"/>
+    <mergeCell ref="F76:J76"/>
     <mergeCell ref="B68:C68"/>
     <mergeCell ref="G68:I68"/>
     <mergeCell ref="B69:C69"/>
@@ -4724,25 +4635,115 @@
     <mergeCell ref="G66:I66"/>
     <mergeCell ref="B67:C67"/>
     <mergeCell ref="G67:I67"/>
-    <mergeCell ref="A80:A82"/>
-    <mergeCell ref="F80:J80"/>
-    <mergeCell ref="F81:J81"/>
-    <mergeCell ref="F82:J82"/>
-    <mergeCell ref="A77:A79"/>
-    <mergeCell ref="B79:E79"/>
-    <mergeCell ref="F79:J79"/>
-    <mergeCell ref="B73:E73"/>
-    <mergeCell ref="F73:J73"/>
-    <mergeCell ref="B77:E77"/>
-    <mergeCell ref="F77:J77"/>
-    <mergeCell ref="B78:E78"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="F74:J74"/>
-    <mergeCell ref="B75:E75"/>
-    <mergeCell ref="F75:J75"/>
-    <mergeCell ref="B76:E76"/>
-    <mergeCell ref="F76:J76"/>
+    <mergeCell ref="A50:A59"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="F50:I50"/>
+    <mergeCell ref="B51:E51"/>
+    <mergeCell ref="F51:I51"/>
+    <mergeCell ref="B52:E52"/>
+    <mergeCell ref="F52:I52"/>
+    <mergeCell ref="B53:E53"/>
+    <mergeCell ref="F53:I53"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="F54:I54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="F55:I55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="F56:I56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="F57:I57"/>
+    <mergeCell ref="B58:E58"/>
+    <mergeCell ref="F58:I58"/>
+    <mergeCell ref="B59:E59"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="A40:A49"/>
+    <mergeCell ref="B40:E40"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="B43:E43"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="B44:E44"/>
+    <mergeCell ref="F44:I44"/>
+    <mergeCell ref="B45:E45"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="F46:I46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="F47:I47"/>
+    <mergeCell ref="B48:E48"/>
+    <mergeCell ref="F48:I48"/>
+    <mergeCell ref="B49:E49"/>
+    <mergeCell ref="F49:I49"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="G36:J36"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="G22:J22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="G23:J23"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="G24:J24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="G19:J19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="A30:E30"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A72:C72"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="A13:A21"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="G21:J21"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="I9:J9"/>
   </mergeCells>
   <phoneticPr fontId="13" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>